<commit_message>
Hemos conseguido rellenar la columna uds. objetivo semana pasada
</commit_message>
<xml_diff>
--- a/data/output/Pedido_Semana_08_09022026_deco_interior.xlsx
+++ b/data/output/Pedido_Semana_08_09022026_deco_interior.xlsx
@@ -1135,7 +1135,7 @@
         <v>2</v>
       </c>
       <c r="Q8" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="3" t="n">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="Q10" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="3" t="n">
         <v>0</v>
@@ -1378,7 +1378,7 @@
         <v>2</v>
       </c>
       <c r="Q11" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="3" t="n">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>7</v>
       </c>
       <c r="Q16" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="3" t="n">
         <v>0</v>
@@ -1864,7 +1864,7 @@
         <v>3</v>
       </c>
       <c r="Q17" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R17" s="3" t="n">
         <v>0</v>
@@ -1945,7 +1945,7 @@
         <v>6</v>
       </c>
       <c r="Q18" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="3" t="n">
         <v>0</v>
@@ -2026,7 +2026,7 @@
         <v>3</v>
       </c>
       <c r="Q19" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R19" s="3" t="n">
         <v>0</v>
@@ -2431,7 +2431,7 @@
         <v>3</v>
       </c>
       <c r="Q24" s="2" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R24" s="3" t="n">
         <v>0</v>
@@ -2755,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="Q28" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="3" t="n">
         <v>0</v>
@@ -2998,7 +2998,7 @@
         <v>4</v>
       </c>
       <c r="Q31" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" s="3" t="n">
         <v>0</v>
@@ -3565,7 +3565,7 @@
         <v>2</v>
       </c>
       <c r="Q38" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" s="3" t="n">
         <v>0</v>
@@ -3727,7 +3727,7 @@
         <v>2</v>
       </c>
       <c r="Q40" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="3" t="n">
         <v>0</v>
@@ -3808,7 +3808,7 @@
         <v>3</v>
       </c>
       <c r="Q41" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R41" s="3" t="n">
         <v>0</v>
@@ -4294,7 +4294,7 @@
         <v>2</v>
       </c>
       <c r="Q47" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R47" s="3" t="n">
         <v>0</v>
@@ -4375,7 +4375,7 @@
         <v>2</v>
       </c>
       <c r="Q48" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="3" t="n">
         <v>0</v>
@@ -5347,7 +5347,7 @@
         <v>2</v>
       </c>
       <c r="Q60" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R60" s="3" t="n">
         <v>0</v>
@@ -5509,7 +5509,7 @@
         <v>6</v>
       </c>
       <c r="Q62" s="2" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R62" s="3" t="n">
         <v>0</v>
@@ -5914,7 +5914,7 @@
         <v>2</v>
       </c>
       <c r="Q67" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R67" s="3" t="n">
         <v>0</v>
@@ -5995,7 +5995,7 @@
         <v>4</v>
       </c>
       <c r="Q68" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R68" s="3" t="n">
         <v>0</v>
@@ -6076,7 +6076,7 @@
         <v>4</v>
       </c>
       <c r="Q69" s="2" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R69" s="3" t="n">
         <v>0</v>
@@ -6319,7 +6319,7 @@
         <v>4</v>
       </c>
       <c r="Q72" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R72" s="3" t="n">
         <v>0</v>
@@ -7696,7 +7696,7 @@
         <v>2</v>
       </c>
       <c r="Q89" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R89" s="3" t="n">
         <v>0</v>
@@ -7777,7 +7777,7 @@
         <v>7</v>
       </c>
       <c r="Q90" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R90" s="3" t="n">
         <v>0</v>
@@ -8182,7 +8182,7 @@
         <v>3</v>
       </c>
       <c r="Q95" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R95" s="3" t="n">
         <v>0</v>
@@ -8263,7 +8263,7 @@
         <v>3</v>
       </c>
       <c r="Q96" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R96" s="3" t="n">
         <v>0</v>

</xml_diff>